<commit_message>
Parser fonctionel? je crois bien
</commit_message>
<xml_diff>
--- a/doc/grammar_doc/First_follow.xlsx
+++ b/doc/grammar_doc/First_follow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\alex\MA1\infof413_pascalmaispresque\doc\grammar_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0088220E-CF7B-4FEE-810F-FAC837577BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9761DB-3653-4BD5-BD1A-F8665F3D6EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6672" yWindow="7956" windowWidth="23040" windowHeight="12204" xr2:uid="{5599AC06-8F86-4CD3-AB13-3F69618E0F1C}"/>
+    <workbookView xWindow="7668" yWindow="4068" windowWidth="23040" windowHeight="12204" xr2:uid="{5599AC06-8F86-4CD3-AB13-3F69618E0F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -98,36 +98,24 @@
     <t>(, -, [VARNAME], [NUMBER]</t>
   </si>
   <si>
-    <t>…,else, end, ), *, /,  =, &lt;, and, or, then</t>
-  </si>
-  <si>
     <t>ExprArith'</t>
   </si>
   <si>
     <t>+, -, ɛ</t>
   </si>
   <si>
-    <t>…,else, end ), *, /,  =, &lt;, and, or, then</t>
-  </si>
-  <si>
     <t>MultExpr</t>
   </si>
   <si>
     <t>(, - , [VARNAME], [NUMBER]</t>
   </si>
   <si>
-    <t>…,else, end ), *, /,  =, &lt;, and,or, then +, -</t>
-  </si>
-  <si>
     <t>MultExpr'</t>
   </si>
   <si>
     <t>*, /, ɛ</t>
   </si>
   <si>
-    <t>…,else, end ), *, /,  =, &lt;, and, or, then, +, -</t>
-  </si>
-  <si>
     <t>Term</t>
   </si>
   <si>
@@ -213,6 +201,18 @@
   </si>
   <si>
     <t>read</t>
+  </si>
+  <si>
+    <t>…,else, end, ), *, /,  =, &lt;, and, or, then, do</t>
+  </si>
+  <si>
+    <t>…,else, end ), *, /,  =, &lt;, and, or, then, do</t>
+  </si>
+  <si>
+    <t>…,else, end ), *, /,  =, &lt;, and,or, then +, -, do</t>
+  </si>
+  <si>
+    <t>…,else, end ), *, /,  =, &lt;, and, or, then, +, -, do</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C26"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,81 +937,81 @@
         <v>19</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" s="9" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>17</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>7</v>
@@ -1030,76 +1030,76 @@
     </row>
     <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>19</v>
@@ -1107,10 +1107,10 @@
     </row>
     <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>17</v>
@@ -1118,10 +1118,10 @@
     </row>
     <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>17</v>
@@ -1129,10 +1129,10 @@
     </row>
     <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>17</v>

</xml_diff>